<commit_message>
Added some figures to design chapter, began writing it.
</commit_message>
<xml_diff>
--- a/_notes/thesis progress.xlsx
+++ b/_notes/thesis progress.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="28">
   <si>
     <t>Days left</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>2.2 data visualization</t>
+  </si>
+  <si>
+    <t>(Design) 2.2 data viz</t>
   </si>
 </sst>
 </file>
@@ -504,7 +507,7 @@
   <dimension ref="A1:P46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -868,16 +871,22 @@
         <f t="shared" si="2"/>
         <v>42.857142857142875</v>
       </c>
+      <c r="E12">
+        <v>40</v>
+      </c>
       <c r="F12">
         <f t="shared" si="3"/>
-        <v>-40</v>
+        <v>0</v>
       </c>
       <c r="G12" s="2">
         <f t="shared" si="1"/>
-        <v>-42.857142857142875</v>
+        <v>-2.8571428571428754</v>
+      </c>
+      <c r="H12" t="s">
+        <v>26</v>
       </c>
       <c r="J12">
-        <f t="shared" si="4"/>
+        <f>J11+2</f>
         <v>44</v>
       </c>
     </row>
@@ -896,13 +905,19 @@
         <f t="shared" si="2"/>
         <v>44.342857142857163</v>
       </c>
+      <c r="E13">
+        <v>44</v>
+      </c>
       <c r="F13">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G13" s="2">
         <f t="shared" si="1"/>
-        <v>-44.342857142857163</v>
+        <v>-0.34285714285716296</v>
+      </c>
+      <c r="H13" t="s">
+        <v>27</v>
       </c>
       <c r="J13">
         <f t="shared" si="4"/>
@@ -926,7 +941,7 @@
       </c>
       <c r="F14">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-44</v>
       </c>
       <c r="G14" s="2">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
Wrote about webmapper in design.
</commit_message>
<xml_diff>
--- a/_notes/thesis progress.xlsx
+++ b/_notes/thesis progress.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="28">
   <si>
     <t>Days left</t>
   </si>
@@ -154,8 +154,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -168,13 +170,15 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -507,7 +511,7 @@
   <dimension ref="A1:P46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -939,13 +943,19 @@
         <f t="shared" si="2"/>
         <v>45.82857142857145</v>
       </c>
+      <c r="E14">
+        <v>44</v>
+      </c>
       <c r="F14">
         <f t="shared" si="3"/>
-        <v>-44</v>
+        <v>0</v>
       </c>
       <c r="G14" s="2">
         <f t="shared" si="1"/>
-        <v>-45.82857142857145</v>
+        <v>-1.8285714285714505</v>
+      </c>
+      <c r="H14" t="s">
+        <v>27</v>
       </c>
       <c r="I14" t="s">
         <v>24</v>
@@ -970,13 +980,19 @@
         <f t="shared" si="2"/>
         <v>47.314285714285738</v>
       </c>
+      <c r="E15">
+        <v>46</v>
+      </c>
       <c r="F15">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G15" s="2">
         <f t="shared" si="1"/>
-        <v>-47.314285714285738</v>
+        <v>-1.314285714285738</v>
+      </c>
+      <c r="H15" t="s">
+        <v>27</v>
       </c>
       <c r="J15">
         <f t="shared" si="4"/>
@@ -1015,7 +1031,7 @@
       </c>
       <c r="F16">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-46</v>
       </c>
       <c r="G16" s="2">
         <f t="shared" si="1"/>
@@ -1751,6 +1767,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Continued work describing list view.
</commit_message>
<xml_diff>
--- a/_notes/thesis progress.xlsx
+++ b/_notes/thesis progress.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15620" tabRatio="500"/>
+    <workbookView xWindow="5720" yWindow="1460" windowWidth="21520" windowHeight="18260" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="28">
   <si>
     <t>Days left</t>
   </si>
@@ -511,7 +511,7 @@
   <dimension ref="A1:P46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -584,7 +584,7 @@
       </c>
       <c r="D3" s="2">
         <f t="shared" ref="D3:D36" si="2">D2+P$16</f>
-        <v>29.485714285714288</v>
+        <v>30</v>
       </c>
       <c r="E3">
         <v>28</v>
@@ -595,7 +595,7 @@
       </c>
       <c r="G3" s="2">
         <f t="shared" si="1"/>
-        <v>-1.4857142857142875</v>
+        <v>-2</v>
       </c>
       <c r="H3" t="s">
         <v>10</v>
@@ -614,7 +614,7 @@
       </c>
       <c r="D4" s="2">
         <f t="shared" si="2"/>
-        <v>30.971428571428575</v>
+        <v>32</v>
       </c>
       <c r="E4">
         <v>30</v>
@@ -625,7 +625,7 @@
       </c>
       <c r="G4" s="2">
         <f t="shared" si="1"/>
-        <v>-0.97142857142857508</v>
+        <v>-2</v>
       </c>
       <c r="H4" t="s">
         <v>11</v>
@@ -644,7 +644,7 @@
       </c>
       <c r="D5" s="2">
         <f t="shared" si="2"/>
-        <v>32.457142857142863</v>
+        <v>34</v>
       </c>
       <c r="E5">
         <f>E4</f>
@@ -656,7 +656,7 @@
       </c>
       <c r="G5" s="2">
         <f t="shared" si="1"/>
-        <v>-2.4571428571428626</v>
+        <v>-4</v>
       </c>
       <c r="H5" t="s">
         <v>11</v>
@@ -675,7 +675,7 @@
       </c>
       <c r="D6" s="2">
         <f t="shared" si="2"/>
-        <v>33.94285714285715</v>
+        <v>36</v>
       </c>
       <c r="E6">
         <v>32</v>
@@ -685,7 +685,7 @@
       </c>
       <c r="G6" s="2">
         <f t="shared" si="1"/>
-        <v>-1.9428571428571502</v>
+        <v>-4</v>
       </c>
       <c r="H6" t="s">
         <v>11</v>
@@ -704,7 +704,7 @@
       </c>
       <c r="D7" s="2">
         <f t="shared" si="2"/>
-        <v>35.428571428571438</v>
+        <v>38</v>
       </c>
       <c r="E7">
         <v>34</v>
@@ -715,13 +715,10 @@
       </c>
       <c r="G7" s="2">
         <f t="shared" si="1"/>
-        <v>-1.4285714285714377</v>
+        <v>-4</v>
       </c>
       <c r="H7" t="s">
         <v>21</v>
-      </c>
-      <c r="J7">
-        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -737,7 +734,7 @@
       </c>
       <c r="D8" s="2">
         <f t="shared" si="2"/>
-        <v>36.914285714285725</v>
+        <v>40</v>
       </c>
       <c r="E8">
         <v>35</v>
@@ -748,14 +745,10 @@
       </c>
       <c r="G8" s="2">
         <f t="shared" si="1"/>
-        <v>-1.9142857142857252</v>
+        <v>-5</v>
       </c>
       <c r="H8" t="s">
         <v>21</v>
-      </c>
-      <c r="J8">
-        <f>J7+2</f>
-        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -771,7 +764,7 @@
       </c>
       <c r="D9" s="2">
         <f t="shared" si="2"/>
-        <v>38.400000000000013</v>
+        <v>42</v>
       </c>
       <c r="E9">
         <v>36</v>
@@ -782,14 +775,10 @@
       </c>
       <c r="G9" s="2">
         <f t="shared" si="1"/>
-        <v>-2.4000000000000128</v>
+        <v>-6</v>
       </c>
       <c r="H9" t="s">
         <v>21</v>
-      </c>
-      <c r="J9">
-        <f t="shared" ref="J9:J30" si="4">J8+2</f>
-        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -805,7 +794,7 @@
       </c>
       <c r="D10" s="2">
         <f t="shared" si="2"/>
-        <v>39.8857142857143</v>
+        <v>44</v>
       </c>
       <c r="E10">
         <v>37</v>
@@ -816,14 +805,10 @@
       </c>
       <c r="G10" s="2">
         <f t="shared" si="1"/>
-        <v>-2.8857142857143003</v>
+        <v>-7</v>
       </c>
       <c r="H10" t="s">
         <v>21</v>
-      </c>
-      <c r="J10">
-        <f t="shared" si="4"/>
-        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -839,7 +824,7 @@
       </c>
       <c r="D11" s="2">
         <f t="shared" si="2"/>
-        <v>41.371428571428588</v>
+        <v>46</v>
       </c>
       <c r="E11">
         <v>40</v>
@@ -850,14 +835,10 @@
       </c>
       <c r="G11" s="2">
         <f t="shared" si="1"/>
-        <v>-1.3714285714285879</v>
+        <v>-6</v>
       </c>
       <c r="H11" t="s">
         <v>26</v>
-      </c>
-      <c r="J11">
-        <f t="shared" si="4"/>
-        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:16">
@@ -873,7 +854,7 @@
       </c>
       <c r="D12" s="2">
         <f t="shared" si="2"/>
-        <v>42.857142857142875</v>
+        <v>48</v>
       </c>
       <c r="E12">
         <v>40</v>
@@ -884,14 +865,10 @@
       </c>
       <c r="G12" s="2">
         <f t="shared" si="1"/>
-        <v>-2.8571428571428754</v>
+        <v>-8</v>
       </c>
       <c r="H12" t="s">
         <v>26</v>
-      </c>
-      <c r="J12">
-        <f>J11+2</f>
-        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:16">
@@ -907,7 +884,7 @@
       </c>
       <c r="D13" s="2">
         <f t="shared" si="2"/>
-        <v>44.342857142857163</v>
+        <v>50</v>
       </c>
       <c r="E13">
         <v>44</v>
@@ -918,14 +895,10 @@
       </c>
       <c r="G13" s="2">
         <f t="shared" si="1"/>
-        <v>-0.34285714285716296</v>
+        <v>-6</v>
       </c>
       <c r="H13" t="s">
         <v>27</v>
-      </c>
-      <c r="J13">
-        <f t="shared" si="4"/>
-        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:16">
@@ -941,7 +914,7 @@
       </c>
       <c r="D14" s="2">
         <f t="shared" si="2"/>
-        <v>45.82857142857145</v>
+        <v>52</v>
       </c>
       <c r="E14">
         <v>44</v>
@@ -952,17 +925,13 @@
       </c>
       <c r="G14" s="2">
         <f t="shared" si="1"/>
-        <v>-1.8285714285714505</v>
+        <v>-8</v>
       </c>
       <c r="H14" t="s">
         <v>27</v>
       </c>
       <c r="I14" t="s">
         <v>24</v>
-      </c>
-      <c r="J14">
-        <f t="shared" si="4"/>
-        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:16">
@@ -978,7 +947,7 @@
       </c>
       <c r="D15" s="2">
         <f t="shared" si="2"/>
-        <v>47.314285714285738</v>
+        <v>54</v>
       </c>
       <c r="E15">
         <v>46</v>
@@ -989,14 +958,10 @@
       </c>
       <c r="G15" s="2">
         <f t="shared" si="1"/>
-        <v>-1.314285714285738</v>
+        <v>-8</v>
       </c>
       <c r="H15" t="s">
         <v>27</v>
-      </c>
-      <c r="J15">
-        <f t="shared" si="4"/>
-        <v>50</v>
       </c>
       <c r="L15" t="s">
         <v>2</v>
@@ -1027,39 +992,42 @@
       </c>
       <c r="D16" s="2">
         <f t="shared" si="2"/>
-        <v>48.800000000000026</v>
+        <v>56</v>
+      </c>
+      <c r="E16">
+        <v>46</v>
       </c>
       <c r="F16">
         <f t="shared" si="3"/>
-        <v>-46</v>
+        <v>0</v>
       </c>
       <c r="G16" s="2">
         <f t="shared" si="1"/>
-        <v>-48.800000000000026</v>
-      </c>
-      <c r="J16">
-        <f t="shared" si="4"/>
-        <v>52</v>
+        <v>-10</v>
+      </c>
+      <c r="H16" t="s">
+        <v>27</v>
       </c>
       <c r="L16">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="M16">
         <v>80</v>
       </c>
       <c r="N16">
-        <v>35</v>
+        <f>24-7</f>
+        <v>17</v>
       </c>
       <c r="O16">
         <f>M16-L16</f>
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="P16">
         <f>O16/N16</f>
-        <v>1.4857142857142858</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1072,7 +1040,10 @@
       </c>
       <c r="D17" s="2">
         <f t="shared" si="2"/>
-        <v>50.285714285714313</v>
+        <v>58</v>
+      </c>
+      <c r="E17">
+        <v>46</v>
       </c>
       <c r="F17">
         <f t="shared" si="3"/>
@@ -1080,14 +1051,13 @@
       </c>
       <c r="G17" s="2">
         <f t="shared" si="1"/>
-        <v>-50.285714285714313</v>
-      </c>
-      <c r="J17">
-        <f t="shared" si="4"/>
-        <v>54</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10">
+        <v>-12</v>
+      </c>
+      <c r="H17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -1100,7 +1070,10 @@
       </c>
       <c r="D18" s="2">
         <f t="shared" si="2"/>
-        <v>51.771428571428601</v>
+        <v>60</v>
+      </c>
+      <c r="E18">
+        <v>46</v>
       </c>
       <c r="F18">
         <f t="shared" si="3"/>
@@ -1108,14 +1081,13 @@
       </c>
       <c r="G18" s="2">
         <f t="shared" si="1"/>
-        <v>-51.771428571428601</v>
-      </c>
-      <c r="J18">
-        <f t="shared" si="4"/>
-        <v>56</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10">
+        <v>-14</v>
+      </c>
+      <c r="H18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -1128,7 +1100,10 @@
       </c>
       <c r="D19" s="2">
         <f t="shared" si="2"/>
-        <v>53.257142857142888</v>
+        <v>62</v>
+      </c>
+      <c r="E19">
+        <v>46</v>
       </c>
       <c r="F19">
         <f t="shared" si="3"/>
@@ -1136,14 +1111,13 @@
       </c>
       <c r="G19" s="2">
         <f t="shared" si="1"/>
-        <v>-53.257142857142888</v>
-      </c>
-      <c r="J19">
-        <f t="shared" si="4"/>
-        <v>58</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10">
+        <v>-16</v>
+      </c>
+      <c r="H19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20" t="s">
         <v>13</v>
       </c>
@@ -1156,22 +1130,21 @@
       </c>
       <c r="D20" s="2">
         <f t="shared" si="2"/>
-        <v>54.742857142857176</v>
+        <v>64</v>
+      </c>
+      <c r="E20">
+        <v>49</v>
       </c>
       <c r="F20">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G20" s="2">
         <f t="shared" si="1"/>
-        <v>-54.742857142857176</v>
-      </c>
-      <c r="J20">
-        <f t="shared" si="4"/>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10">
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -1184,22 +1157,18 @@
       </c>
       <c r="D21" s="2">
         <f t="shared" si="2"/>
-        <v>56.228571428571463</v>
+        <v>66</v>
       </c>
       <c r="F21">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-49</v>
       </c>
       <c r="G21" s="2">
         <f t="shared" si="1"/>
-        <v>-56.228571428571463</v>
-      </c>
-      <c r="J21">
-        <f t="shared" si="4"/>
-        <v>62</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10">
+        <v>-66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
       <c r="A22" t="s">
         <v>18</v>
       </c>
@@ -1212,7 +1181,7 @@
       </c>
       <c r="D22" s="2">
         <f t="shared" si="2"/>
-        <v>57.714285714285751</v>
+        <v>68</v>
       </c>
       <c r="F22">
         <f t="shared" si="3"/>
@@ -1220,14 +1189,10 @@
       </c>
       <c r="G22" s="2">
         <f t="shared" si="1"/>
-        <v>-57.714285714285751</v>
-      </c>
-      <c r="J22">
-        <f t="shared" si="4"/>
-        <v>64</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10">
+        <v>-68</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
       <c r="A23" t="s">
         <v>17</v>
       </c>
@@ -1240,7 +1205,7 @@
       </c>
       <c r="D23" s="2">
         <f t="shared" si="2"/>
-        <v>59.200000000000038</v>
+        <v>70</v>
       </c>
       <c r="F23">
         <f t="shared" si="3"/>
@@ -1248,14 +1213,10 @@
       </c>
       <c r="G23" s="2">
         <f t="shared" si="1"/>
-        <v>-59.200000000000038</v>
-      </c>
-      <c r="J23">
-        <f t="shared" si="4"/>
-        <v>66</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10">
+        <v>-70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24" t="s">
         <v>16</v>
       </c>
@@ -1268,7 +1229,7 @@
       </c>
       <c r="D24" s="2">
         <f t="shared" si="2"/>
-        <v>60.685714285714326</v>
+        <v>72</v>
       </c>
       <c r="F24">
         <f t="shared" si="3"/>
@@ -1276,14 +1237,10 @@
       </c>
       <c r="G24" s="2">
         <f t="shared" si="1"/>
-        <v>-60.685714285714326</v>
-      </c>
-      <c r="J24">
-        <f t="shared" si="4"/>
-        <v>68</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10">
+        <v>-72</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25" t="s">
         <v>15</v>
       </c>
@@ -1296,7 +1253,7 @@
       </c>
       <c r="D25" s="2">
         <f t="shared" si="2"/>
-        <v>62.171428571428613</v>
+        <v>74</v>
       </c>
       <c r="F25">
         <f t="shared" si="3"/>
@@ -1304,17 +1261,13 @@
       </c>
       <c r="G25" s="2">
         <f t="shared" si="1"/>
-        <v>-62.171428571428613</v>
+        <v>-74</v>
       </c>
       <c r="I25" t="s">
         <v>25</v>
       </c>
-      <c r="J25">
-        <f t="shared" si="4"/>
-        <v>70</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10">
+    </row>
+    <row r="26" spans="1:9">
       <c r="A26" t="s">
         <v>14</v>
       </c>
@@ -1327,7 +1280,7 @@
       </c>
       <c r="D26" s="2">
         <f t="shared" si="2"/>
-        <v>63.657142857142901</v>
+        <v>76</v>
       </c>
       <c r="F26">
         <f t="shared" si="3"/>
@@ -1335,14 +1288,10 @@
       </c>
       <c r="G26" s="2">
         <f t="shared" si="1"/>
-        <v>-63.657142857142901</v>
-      </c>
-      <c r="J26">
-        <f t="shared" si="4"/>
-        <v>72</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10">
+        <v>-76</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
       <c r="A27" t="s">
         <v>13</v>
       </c>
@@ -1355,7 +1304,7 @@
       </c>
       <c r="D27" s="2">
         <f t="shared" si="2"/>
-        <v>65.142857142857181</v>
+        <v>78</v>
       </c>
       <c r="F27">
         <f t="shared" si="3"/>
@@ -1363,14 +1312,10 @@
       </c>
       <c r="G27" s="2">
         <f t="shared" si="1"/>
-        <v>-65.142857142857181</v>
-      </c>
-      <c r="J27">
-        <f t="shared" si="4"/>
-        <v>74</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10">
+        <v>-78</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
       <c r="A28" t="s">
         <v>12</v>
       </c>
@@ -1383,7 +1328,7 @@
       </c>
       <c r="D28" s="2">
         <f t="shared" si="2"/>
-        <v>66.628571428571462</v>
+        <v>80</v>
       </c>
       <c r="F28">
         <f t="shared" si="3"/>
@@ -1391,14 +1336,10 @@
       </c>
       <c r="G28" s="2">
         <f t="shared" si="1"/>
-        <v>-66.628571428571462</v>
-      </c>
-      <c r="J28">
-        <f t="shared" si="4"/>
-        <v>76</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10">
+        <v>-80</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
       <c r="A29" t="s">
         <v>18</v>
       </c>
@@ -1411,7 +1352,7 @@
       </c>
       <c r="D29" s="2">
         <f t="shared" si="2"/>
-        <v>68.114285714285742</v>
+        <v>82</v>
       </c>
       <c r="F29">
         <f t="shared" si="3"/>
@@ -1419,14 +1360,10 @@
       </c>
       <c r="G29" s="2">
         <f t="shared" si="1"/>
-        <v>-68.114285714285742</v>
-      </c>
-      <c r="J29">
-        <f t="shared" si="4"/>
-        <v>78</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10">
+        <v>-82</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
       <c r="A30" t="s">
         <v>17</v>
       </c>
@@ -1439,7 +1376,7 @@
       </c>
       <c r="D30" s="2">
         <f t="shared" si="2"/>
-        <v>69.600000000000023</v>
+        <v>84</v>
       </c>
       <c r="F30">
         <f t="shared" si="3"/>
@@ -1447,14 +1384,10 @@
       </c>
       <c r="G30" s="2">
         <f t="shared" si="1"/>
-        <v>-69.600000000000023</v>
-      </c>
-      <c r="J30">
-        <f t="shared" si="4"/>
-        <v>80</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10">
+        <v>-84</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
       <c r="A31" t="s">
         <v>16</v>
       </c>
@@ -1467,7 +1400,7 @@
       </c>
       <c r="D31" s="2">
         <f t="shared" si="2"/>
-        <v>71.085714285714303</v>
+        <v>86</v>
       </c>
       <c r="F31">
         <f t="shared" si="3"/>
@@ -1475,10 +1408,10 @@
       </c>
       <c r="G31" s="2">
         <f t="shared" si="1"/>
-        <v>-71.085714285714303</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10">
+        <v>-86</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
       <c r="A32" t="s">
         <v>15</v>
       </c>
@@ -1491,7 +1424,7 @@
       </c>
       <c r="D32" s="2">
         <f t="shared" si="2"/>
-        <v>72.571428571428584</v>
+        <v>88</v>
       </c>
       <c r="F32">
         <f t="shared" si="3"/>
@@ -1499,7 +1432,7 @@
       </c>
       <c r="G32" s="2">
         <f t="shared" si="1"/>
-        <v>-72.571428571428584</v>
+        <v>-88</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -1515,7 +1448,7 @@
       </c>
       <c r="D33" s="2">
         <f t="shared" si="2"/>
-        <v>74.057142857142864</v>
+        <v>90</v>
       </c>
       <c r="F33">
         <f t="shared" si="3"/>
@@ -1523,7 +1456,7 @@
       </c>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
-        <v>-74.057142857142864</v>
+        <v>-90</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -1539,7 +1472,7 @@
       </c>
       <c r="D34" s="2">
         <f t="shared" si="2"/>
-        <v>75.542857142857144</v>
+        <v>92</v>
       </c>
       <c r="F34">
         <f t="shared" si="3"/>
@@ -1547,7 +1480,7 @@
       </c>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
-        <v>-75.542857142857144</v>
+        <v>-92</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -1563,7 +1496,7 @@
       </c>
       <c r="D35" s="2">
         <f>D34+P$16</f>
-        <v>77.028571428571425</v>
+        <v>94</v>
       </c>
       <c r="F35">
         <f t="shared" si="3"/>
@@ -1571,7 +1504,7 @@
       </c>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
-        <v>-77.028571428571425</v>
+        <v>-94</v>
       </c>
     </row>
     <row r="36" spans="1:9">
@@ -1587,7 +1520,7 @@
       </c>
       <c r="D36" s="2">
         <f t="shared" si="2"/>
-        <v>78.514285714285705</v>
+        <v>96</v>
       </c>
       <c r="F36">
         <f t="shared" si="3"/>
@@ -1595,7 +1528,7 @@
       </c>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
-        <v>-78.514285714285705</v>
+        <v>-96</v>
       </c>
       <c r="I36" t="s">
         <v>22</v>
@@ -1767,7 +1700,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Finished graphical part of background!
</commit_message>
<xml_diff>
--- a/_notes/thesis progress.xlsx
+++ b/_notes/thesis progress.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="-40" windowWidth="21520" windowHeight="18260" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -96,16 +96,16 @@
     <t>design</t>
   </si>
   <si>
-    <t>evaluation</t>
-  </si>
-  <si>
     <t>2.2 data visualization</t>
   </si>
   <si>
     <t>(Design) 2.2 data viz</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <t>Evaluation</t>
+  </si>
+  <si>
+    <t>Design</t>
   </si>
 </sst>
 </file>
@@ -517,8 +517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -591,7 +591,7 @@
       </c>
       <c r="D3" s="2">
         <f t="shared" ref="D3:D36" si="2">D2+P$16</f>
-        <v>30</v>
+        <v>29.8</v>
       </c>
       <c r="E3">
         <v>28</v>
@@ -602,7 +602,7 @@
       </c>
       <c r="G3" s="2">
         <f t="shared" si="1"/>
-        <v>-2</v>
+        <v>-1.8000000000000007</v>
       </c>
       <c r="H3" t="s">
         <v>10</v>
@@ -621,7 +621,7 @@
       </c>
       <c r="D4" s="2">
         <f t="shared" si="2"/>
-        <v>32</v>
+        <v>31.6</v>
       </c>
       <c r="E4">
         <v>30</v>
@@ -632,7 +632,7 @@
       </c>
       <c r="G4" s="2">
         <f t="shared" si="1"/>
-        <v>-2</v>
+        <v>-1.6000000000000014</v>
       </c>
       <c r="H4" t="s">
         <v>11</v>
@@ -651,7 +651,7 @@
       </c>
       <c r="D5" s="2">
         <f t="shared" si="2"/>
-        <v>34</v>
+        <v>33.4</v>
       </c>
       <c r="E5">
         <f>E4</f>
@@ -663,7 +663,7 @@
       </c>
       <c r="G5" s="2">
         <f t="shared" si="1"/>
-        <v>-4</v>
+        <v>-3.3999999999999986</v>
       </c>
       <c r="H5" t="s">
         <v>11</v>
@@ -682,7 +682,7 @@
       </c>
       <c r="D6" s="2">
         <f t="shared" si="2"/>
-        <v>36</v>
+        <v>35.199999999999996</v>
       </c>
       <c r="E6">
         <v>32</v>
@@ -692,7 +692,7 @@
       </c>
       <c r="G6" s="2">
         <f t="shared" si="1"/>
-        <v>-4</v>
+        <v>-3.1999999999999957</v>
       </c>
       <c r="H6" t="s">
         <v>11</v>
@@ -711,7 +711,7 @@
       </c>
       <c r="D7" s="2">
         <f t="shared" si="2"/>
-        <v>38</v>
+        <v>36.999999999999993</v>
       </c>
       <c r="E7">
         <v>34</v>
@@ -722,7 +722,7 @@
       </c>
       <c r="G7" s="2">
         <f t="shared" si="1"/>
-        <v>-4</v>
+        <v>-2.9999999999999929</v>
       </c>
       <c r="H7" t="s">
         <v>21</v>
@@ -741,7 +741,7 @@
       </c>
       <c r="D8" s="2">
         <f t="shared" si="2"/>
-        <v>40</v>
+        <v>38.79999999999999</v>
       </c>
       <c r="E8">
         <v>35</v>
@@ -752,7 +752,7 @@
       </c>
       <c r="G8" s="2">
         <f t="shared" si="1"/>
-        <v>-5</v>
+        <v>-3.7999999999999901</v>
       </c>
       <c r="H8" t="s">
         <v>21</v>
@@ -771,7 +771,7 @@
       </c>
       <c r="D9" s="2">
         <f t="shared" si="2"/>
-        <v>42</v>
+        <v>40.599999999999987</v>
       </c>
       <c r="E9">
         <v>36</v>
@@ -782,7 +782,7 @@
       </c>
       <c r="G9" s="2">
         <f t="shared" si="1"/>
-        <v>-6</v>
+        <v>-4.5999999999999872</v>
       </c>
       <c r="H9" t="s">
         <v>21</v>
@@ -801,7 +801,7 @@
       </c>
       <c r="D10" s="2">
         <f t="shared" si="2"/>
-        <v>44</v>
+        <v>42.399999999999984</v>
       </c>
       <c r="E10">
         <v>37</v>
@@ -812,7 +812,7 @@
       </c>
       <c r="G10" s="2">
         <f t="shared" si="1"/>
-        <v>-7</v>
+        <v>-5.3999999999999844</v>
       </c>
       <c r="H10" t="s">
         <v>21</v>
@@ -831,7 +831,7 @@
       </c>
       <c r="D11" s="2">
         <f t="shared" si="2"/>
-        <v>46</v>
+        <v>44.199999999999982</v>
       </c>
       <c r="E11">
         <v>40</v>
@@ -842,10 +842,10 @@
       </c>
       <c r="G11" s="2">
         <f t="shared" si="1"/>
-        <v>-6</v>
+        <v>-4.1999999999999815</v>
       </c>
       <c r="H11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:16">
@@ -861,7 +861,7 @@
       </c>
       <c r="D12" s="2">
         <f t="shared" si="2"/>
-        <v>48</v>
+        <v>45.999999999999979</v>
       </c>
       <c r="E12">
         <v>40</v>
@@ -872,10 +872,10 @@
       </c>
       <c r="G12" s="2">
         <f t="shared" si="1"/>
-        <v>-8</v>
+        <v>-5.9999999999999787</v>
       </c>
       <c r="H12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:16">
@@ -891,7 +891,7 @@
       </c>
       <c r="D13" s="2">
         <f t="shared" si="2"/>
-        <v>50</v>
+        <v>47.799999999999976</v>
       </c>
       <c r="E13">
         <v>44</v>
@@ -902,10 +902,10 @@
       </c>
       <c r="G13" s="2">
         <f t="shared" si="1"/>
-        <v>-6</v>
+        <v>-3.7999999999999758</v>
       </c>
       <c r="H13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:16">
@@ -921,7 +921,7 @@
       </c>
       <c r="D14" s="2">
         <f t="shared" si="2"/>
-        <v>52</v>
+        <v>49.599999999999973</v>
       </c>
       <c r="E14">
         <v>44</v>
@@ -932,10 +932,10 @@
       </c>
       <c r="G14" s="2">
         <f t="shared" si="1"/>
-        <v>-8</v>
+        <v>-5.599999999999973</v>
       </c>
       <c r="H14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I14" t="s">
         <v>24</v>
@@ -954,7 +954,7 @@
       </c>
       <c r="D15" s="2">
         <f t="shared" si="2"/>
-        <v>54</v>
+        <v>51.39999999999997</v>
       </c>
       <c r="E15">
         <v>46</v>
@@ -965,10 +965,10 @@
       </c>
       <c r="G15" s="2">
         <f t="shared" si="1"/>
-        <v>-8</v>
+        <v>-5.3999999999999702</v>
       </c>
       <c r="H15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L15" t="s">
         <v>2</v>
@@ -999,7 +999,7 @@
       </c>
       <c r="D16" s="2">
         <f t="shared" si="2"/>
-        <v>56</v>
+        <v>53.199999999999967</v>
       </c>
       <c r="E16">
         <v>46</v>
@@ -1010,31 +1010,31 @@
       </c>
       <c r="G16" s="2">
         <f t="shared" si="1"/>
-        <v>-10</v>
+        <v>-7.1999999999999673</v>
       </c>
       <c r="H16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L16">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="M16">
         <v>80</v>
       </c>
       <c r="N16">
-        <f>24-7</f>
-        <v>17</v>
+        <f>22-7</f>
+        <v>15</v>
       </c>
       <c r="O16">
         <f>M16-L16</f>
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="P16">
         <f>O16/N16</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1047,7 +1047,7 @@
       </c>
       <c r="D17" s="2">
         <f t="shared" si="2"/>
-        <v>58</v>
+        <v>54.999999999999964</v>
       </c>
       <c r="E17">
         <v>46</v>
@@ -1058,13 +1058,13 @@
       </c>
       <c r="G17" s="2">
         <f t="shared" si="1"/>
-        <v>-12</v>
+        <v>-8.9999999999999645</v>
       </c>
       <c r="H17" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -1077,7 +1077,7 @@
       </c>
       <c r="D18" s="2">
         <f t="shared" si="2"/>
-        <v>60</v>
+        <v>56.799999999999962</v>
       </c>
       <c r="E18">
         <v>46</v>
@@ -1088,13 +1088,13 @@
       </c>
       <c r="G18" s="2">
         <f t="shared" si="1"/>
-        <v>-14</v>
+        <v>-10.799999999999962</v>
       </c>
       <c r="H18" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -1107,7 +1107,7 @@
       </c>
       <c r="D19" s="2">
         <f t="shared" si="2"/>
-        <v>62</v>
+        <v>58.599999999999959</v>
       </c>
       <c r="E19">
         <v>46</v>
@@ -1118,13 +1118,13 @@
       </c>
       <c r="G19" s="2">
         <f t="shared" si="1"/>
-        <v>-16</v>
+        <v>-12.599999999999959</v>
       </c>
       <c r="H19" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20" t="s">
         <v>13</v>
       </c>
@@ -1137,7 +1137,7 @@
       </c>
       <c r="D20" s="2">
         <f t="shared" si="2"/>
-        <v>64</v>
+        <v>60.399999999999956</v>
       </c>
       <c r="E20">
         <v>49</v>
@@ -1148,13 +1148,13 @@
       </c>
       <c r="G20" s="2">
         <f t="shared" si="1"/>
-        <v>-15</v>
+        <v>-11.399999999999956</v>
       </c>
       <c r="H20" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -1167,7 +1167,7 @@
       </c>
       <c r="D21" s="2">
         <f t="shared" si="2"/>
-        <v>66</v>
+        <v>62.199999999999953</v>
       </c>
       <c r="E21">
         <v>53</v>
@@ -1178,10 +1178,10 @@
       </c>
       <c r="G21" s="2">
         <f t="shared" si="1"/>
-        <v>-13</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
+        <v>-9.1999999999999531</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22" t="s">
         <v>18</v>
       </c>
@@ -1194,21 +1194,21 @@
       </c>
       <c r="D22" s="2">
         <f t="shared" si="2"/>
-        <v>68</v>
-      </c>
-      <c r="E22" t="s">
-        <v>28</v>
-      </c>
-      <c r="F22" t="e">
-        <f t="shared" si="3"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G22" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9">
+        <v>63.99999999999995</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="3"/>
+        <v>-53</v>
+      </c>
+      <c r="G22" s="2">
+        <f t="shared" si="1"/>
+        <v>-63.99999999999995</v>
+      </c>
+      <c r="J22">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23" t="s">
         <v>17</v>
       </c>
@@ -1221,18 +1221,22 @@
       </c>
       <c r="D23" s="2">
         <f t="shared" si="2"/>
-        <v>70</v>
-      </c>
-      <c r="F23" t="e">
-        <f t="shared" si="3"/>
-        <v>#VALUE!</v>
+        <v>65.799999999999955</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="G23" s="2">
         <f t="shared" si="1"/>
-        <v>-70</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9">
+        <v>-65.799999999999955</v>
+      </c>
+      <c r="J23">
+        <f>J22+2</f>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24" t="s">
         <v>16</v>
       </c>
@@ -1245,7 +1249,7 @@
       </c>
       <c r="D24" s="2">
         <f t="shared" si="2"/>
-        <v>72</v>
+        <v>67.599999999999952</v>
       </c>
       <c r="F24">
         <f t="shared" si="3"/>
@@ -1253,10 +1257,14 @@
       </c>
       <c r="G24" s="2">
         <f t="shared" si="1"/>
-        <v>-72</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9">
+        <v>-67.599999999999952</v>
+      </c>
+      <c r="J24">
+        <f t="shared" ref="J24:J37" si="4">J23+2</f>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25" t="s">
         <v>15</v>
       </c>
@@ -1269,7 +1277,7 @@
       </c>
       <c r="D25" s="2">
         <f t="shared" si="2"/>
-        <v>74</v>
+        <v>69.399999999999949</v>
       </c>
       <c r="F25">
         <f t="shared" si="3"/>
@@ -1277,13 +1285,17 @@
       </c>
       <c r="G25" s="2">
         <f t="shared" si="1"/>
-        <v>-74</v>
+        <v>-69.399999999999949</v>
       </c>
       <c r="I25" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9">
+        <v>28</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="4"/>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
       <c r="A26" t="s">
         <v>14</v>
       </c>
@@ -1296,7 +1308,7 @@
       </c>
       <c r="D26" s="2">
         <f t="shared" si="2"/>
-        <v>76</v>
+        <v>71.199999999999946</v>
       </c>
       <c r="F26">
         <f t="shared" si="3"/>
@@ -1304,10 +1316,14 @@
       </c>
       <c r="G26" s="2">
         <f t="shared" si="1"/>
-        <v>-76</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9">
+        <v>-71.199999999999946</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="4"/>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
       <c r="A27" t="s">
         <v>13</v>
       </c>
@@ -1320,7 +1336,7 @@
       </c>
       <c r="D27" s="2">
         <f t="shared" si="2"/>
-        <v>78</v>
+        <v>72.999999999999943</v>
       </c>
       <c r="F27">
         <f t="shared" si="3"/>
@@ -1328,10 +1344,14 @@
       </c>
       <c r="G27" s="2">
         <f t="shared" si="1"/>
-        <v>-78</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9">
+        <v>-72.999999999999943</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="4"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
       <c r="A28" t="s">
         <v>12</v>
       </c>
@@ -1344,7 +1364,7 @@
       </c>
       <c r="D28" s="2">
         <f t="shared" si="2"/>
-        <v>80</v>
+        <v>74.79999999999994</v>
       </c>
       <c r="F28">
         <f t="shared" si="3"/>
@@ -1352,10 +1372,14 @@
       </c>
       <c r="G28" s="2">
         <f t="shared" si="1"/>
-        <v>-80</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9">
+        <v>-74.79999999999994</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="4"/>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
       <c r="A29" t="s">
         <v>18</v>
       </c>
@@ -1368,7 +1392,7 @@
       </c>
       <c r="D29" s="2">
         <f t="shared" si="2"/>
-        <v>82</v>
+        <v>76.599999999999937</v>
       </c>
       <c r="F29">
         <f t="shared" si="3"/>
@@ -1376,10 +1400,14 @@
       </c>
       <c r="G29" s="2">
         <f t="shared" si="1"/>
-        <v>-82</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9">
+        <v>-76.599999999999937</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="4"/>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
       <c r="A30" t="s">
         <v>17</v>
       </c>
@@ -1392,7 +1420,7 @@
       </c>
       <c r="D30" s="2">
         <f t="shared" si="2"/>
-        <v>84</v>
+        <v>78.399999999999935</v>
       </c>
       <c r="F30">
         <f t="shared" si="3"/>
@@ -1400,10 +1428,14 @@
       </c>
       <c r="G30" s="2">
         <f t="shared" si="1"/>
-        <v>-84</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9">
+        <v>-78.399999999999935</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="4"/>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
       <c r="A31" t="s">
         <v>16</v>
       </c>
@@ -1416,7 +1448,7 @@
       </c>
       <c r="D31" s="2">
         <f t="shared" si="2"/>
-        <v>86</v>
+        <v>80.199999999999932</v>
       </c>
       <c r="F31">
         <f t="shared" si="3"/>
@@ -1424,10 +1456,14 @@
       </c>
       <c r="G31" s="2">
         <f t="shared" si="1"/>
-        <v>-86</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9">
+        <v>-80.199999999999932</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="4"/>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
       <c r="A32" t="s">
         <v>15</v>
       </c>
@@ -1440,7 +1476,7 @@
       </c>
       <c r="D32" s="2">
         <f t="shared" si="2"/>
-        <v>88</v>
+        <v>81.999999999999929</v>
       </c>
       <c r="F32">
         <f t="shared" si="3"/>
@@ -1448,10 +1484,17 @@
       </c>
       <c r="G32" s="2">
         <f t="shared" si="1"/>
-        <v>-88</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9">
+        <v>-81.999999999999929</v>
+      </c>
+      <c r="I32" t="s">
+        <v>27</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="4"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
       <c r="A33" t="s">
         <v>14</v>
       </c>
@@ -1464,7 +1507,7 @@
       </c>
       <c r="D33" s="2">
         <f t="shared" si="2"/>
-        <v>90</v>
+        <v>83.799999999999926</v>
       </c>
       <c r="F33">
         <f t="shared" si="3"/>
@@ -1472,10 +1515,14 @@
       </c>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
-        <v>-90</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9">
+        <v>-83.799999999999926</v>
+      </c>
+      <c r="J33">
+        <f t="shared" si="4"/>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
       <c r="A34" t="s">
         <v>13</v>
       </c>
@@ -1488,7 +1535,7 @@
       </c>
       <c r="D34" s="2">
         <f t="shared" si="2"/>
-        <v>92</v>
+        <v>85.599999999999923</v>
       </c>
       <c r="F34">
         <f t="shared" si="3"/>
@@ -1496,10 +1543,14 @@
       </c>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
-        <v>-92</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9">
+        <v>-85.599999999999923</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="4"/>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
       <c r="A35" t="s">
         <v>12</v>
       </c>
@@ -1512,7 +1563,7 @@
       </c>
       <c r="D35" s="2">
         <f>D34+P$16</f>
-        <v>94</v>
+        <v>87.39999999999992</v>
       </c>
       <c r="F35">
         <f t="shared" si="3"/>
@@ -1520,10 +1571,14 @@
       </c>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
-        <v>-94</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9">
+        <v>-87.39999999999992</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="4"/>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
       <c r="A36" t="s">
         <v>18</v>
       </c>
@@ -1536,7 +1591,7 @@
       </c>
       <c r="D36" s="2">
         <f t="shared" si="2"/>
-        <v>96</v>
+        <v>89.199999999999918</v>
       </c>
       <c r="F36">
         <f t="shared" si="3"/>
@@ -1544,13 +1599,17 @@
       </c>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
-        <v>-96</v>
+        <v>-89.199999999999918</v>
       </c>
       <c r="I36" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="37" spans="1:9">
+      <c r="J36">
+        <f>J35+2</f>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
       <c r="A37" t="s">
         <v>17</v>
       </c>
@@ -1572,8 +1631,12 @@
         <f t="shared" si="1"/>
         <v>-80</v>
       </c>
-    </row>
-    <row r="38" spans="1:9">
+      <c r="J37">
+        <f t="shared" si="4"/>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
       <c r="A38" t="s">
         <v>16</v>
       </c>
@@ -1594,7 +1657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:10">
       <c r="A39" t="s">
         <v>15</v>
       </c>
@@ -1614,7 +1677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:10">
       <c r="A40" t="s">
         <v>14</v>
       </c>
@@ -1634,7 +1697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:10">
       <c r="A41" t="s">
         <v>13</v>
       </c>
@@ -1654,7 +1717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:10">
       <c r="A42" t="s">
         <v>12</v>
       </c>
@@ -1674,7 +1737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:10">
       <c r="B43">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -1691,7 +1754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:9">
+    <row r="44" spans="1:10">
       <c r="B44">
         <v>0</v>
       </c>
@@ -1707,16 +1770,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:10">
       <c r="C45" s="1"/>
       <c r="G45" s="2"/>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:10">
       <c r="F46" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Shifted work to results chapter.
</commit_message>
<xml_diff>
--- a/_notes/thesis progress.xlsx
+++ b/_notes/thesis progress.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15620" tabRatio="500"/>
+    <workbookView xWindow="-20" yWindow="-20" windowWidth="25580" windowHeight="15620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="30">
   <si>
     <t>Days left</t>
   </si>
@@ -106,6 +106,9 @@
   </si>
   <si>
     <t>Design</t>
+  </si>
+  <si>
+    <t>2.3 GUIs</t>
   </si>
 </sst>
 </file>
@@ -517,8 +520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="CF22" sqref="CF22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1180,6 +1183,9 @@
         <f t="shared" si="1"/>
         <v>-9.1999999999999531</v>
       </c>
+      <c r="H21" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="22" spans="1:10">
       <c r="A22" t="s">
@@ -1196,16 +1202,22 @@
         <f t="shared" si="2"/>
         <v>63.99999999999995</v>
       </c>
+      <c r="E22">
+        <v>57</v>
+      </c>
       <c r="F22">
         <f t="shared" si="3"/>
-        <v>-53</v>
+        <v>4</v>
       </c>
       <c r="G22" s="2">
         <f t="shared" si="1"/>
-        <v>-63.99999999999995</v>
+        <v>-6.9999999999999503</v>
+      </c>
+      <c r="H22" t="s">
+        <v>29</v>
       </c>
       <c r="J22">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -1225,15 +1237,15 @@
       </c>
       <c r="F23">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-57</v>
       </c>
       <c r="G23" s="2">
         <f t="shared" si="1"/>
         <v>-65.799999999999955</v>
       </c>
       <c r="J23">
-        <f>J22+2</f>
-        <v>57</v>
+        <f>J22+4</f>
+        <v>61</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -1261,7 +1273,7 @@
       </c>
       <c r="J24">
         <f t="shared" ref="J24:J37" si="4">J23+2</f>
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -1292,7 +1304,7 @@
       </c>
       <c r="J25">
         <f t="shared" si="4"/>
-        <v>61</v>
+        <v>65</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -1320,7 +1332,7 @@
       </c>
       <c r="J26">
         <f t="shared" si="4"/>
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -1348,7 +1360,7 @@
       </c>
       <c r="J27">
         <f t="shared" si="4"/>
-        <v>65</v>
+        <v>69</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -1376,7 +1388,7 @@
       </c>
       <c r="J28">
         <f t="shared" si="4"/>
-        <v>67</v>
+        <v>71</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -1404,7 +1416,7 @@
       </c>
       <c r="J29">
         <f t="shared" si="4"/>
-        <v>69</v>
+        <v>73</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -1432,7 +1444,7 @@
       </c>
       <c r="J30">
         <f t="shared" si="4"/>
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -1460,7 +1472,7 @@
       </c>
       <c r="J31">
         <f t="shared" si="4"/>
-        <v>73</v>
+        <v>77</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -1491,7 +1503,7 @@
       </c>
       <c r="J32">
         <f t="shared" si="4"/>
-        <v>75</v>
+        <v>79</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -1519,7 +1531,7 @@
       </c>
       <c r="J33">
         <f t="shared" si="4"/>
-        <v>77</v>
+        <v>81</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -1547,7 +1559,7 @@
       </c>
       <c r="J34">
         <f t="shared" si="4"/>
-        <v>79</v>
+        <v>83</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -1575,7 +1587,7 @@
       </c>
       <c r="J35">
         <f t="shared" si="4"/>
-        <v>81</v>
+        <v>85</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -1606,7 +1618,7 @@
       </c>
       <c r="J36">
         <f>J35+2</f>
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -1633,7 +1645,7 @@
       </c>
       <c r="J37">
         <f t="shared" si="4"/>
-        <v>85</v>
+        <v>89</v>
       </c>
     </row>
     <row r="38" spans="1:10">

</xml_diff>

<commit_message>
Lotsa changes. I can't sort em out!
</commit_message>
<xml_diff>
--- a/_notes/thesis progress.xlsx
+++ b/_notes/thesis progress.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="25580" windowHeight="15620" tabRatio="500"/>
+    <workbookView xWindow="-80" yWindow="0" windowWidth="25600" windowHeight="15560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="67">
   <si>
     <t>Days left</t>
   </si>
@@ -109,12 +110,126 @@
   </si>
   <si>
     <t>2.3 GUIs</t>
+  </si>
+  <si>
+    <t>Context and Motivation</t>
+  </si>
+  <si>
+    <t>Project Overview</t>
+  </si>
+  <si>
+    <t>Thesis Overview</t>
+  </si>
+  <si>
+    <t>Contributions</t>
+  </si>
+  <si>
+    <t>Mapping</t>
+  </si>
+  <si>
+    <t>Data Visualization</t>
+  </si>
+  <si>
+    <t>User Interface Design</t>
+  </si>
+  <si>
+    <t>Summary</t>
+  </si>
+  <si>
+    <t>Background</t>
+  </si>
+  <si>
+    <t>libmapper</t>
+  </si>
+  <si>
+    <t>OSC</t>
+  </si>
+  <si>
+    <t>Structure</t>
+  </si>
+  <si>
+    <t>Connection Props</t>
+  </si>
+  <si>
+    <t>libmapper bindings</t>
+  </si>
+  <si>
+    <t>prior interfaces</t>
+  </si>
+  <si>
+    <t>lib variables</t>
+  </si>
+  <si>
+    <t>flexible system</t>
+  </si>
+  <si>
+    <t>interface features</t>
+  </si>
+  <si>
+    <t>extension</t>
+  </si>
+  <si>
+    <t>other features</t>
+  </si>
+  <si>
+    <t>application</t>
+  </si>
+  <si>
+    <t>comparison</t>
+  </si>
+  <si>
+    <t>feedback</t>
+  </si>
+  <si>
+    <t>responsiveness</t>
+  </si>
+  <si>
+    <t>evaluation</t>
+  </si>
+  <si>
+    <t>summary</t>
+  </si>
+  <si>
+    <t>future work</t>
+  </si>
+  <si>
+    <t>Introduction</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>&lt; 0.5</t>
+  </si>
+  <si>
+    <t>&gt; 0.5</t>
+  </si>
+  <si>
+    <t>not started</t>
+  </si>
+  <si>
+    <t>sums</t>
+  </si>
+  <si>
+    <t>Score</t>
+  </si>
+  <si>
+    <t>Goal score</t>
+  </si>
+  <si>
+    <t>Actual Difference</t>
+  </si>
+  <si>
+    <t>Goal Difference</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -151,12 +266,92 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -173,10 +368,27 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -521,7 +733,7 @@
   <dimension ref="A1:P46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="CF22" sqref="CF22"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1235,13 +1447,16 @@
         <f t="shared" si="2"/>
         <v>65.799999999999955</v>
       </c>
+      <c r="E23">
+        <v>62</v>
+      </c>
       <c r="F23">
         <f t="shared" si="3"/>
-        <v>-57</v>
+        <v>5</v>
       </c>
       <c r="G23" s="2">
         <f t="shared" si="1"/>
-        <v>-65.799999999999955</v>
+        <v>-3.7999999999999545</v>
       </c>
       <c r="J23">
         <f>J22+4</f>
@@ -1265,7 +1480,7 @@
       </c>
       <c r="F24">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-62</v>
       </c>
       <c r="G24" s="2">
         <f t="shared" si="1"/>
@@ -1797,4 +2012,647 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:R29"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:18">
+      <c r="D2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G2" t="s">
+        <v>61</v>
+      </c>
+      <c r="N2" t="s">
+        <v>63</v>
+      </c>
+      <c r="O2" t="s">
+        <v>64</v>
+      </c>
+      <c r="P2" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>66</v>
+      </c>
+      <c r="R2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="2:18">
+      <c r="B3" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="5">
+        <v>1</v>
+      </c>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="6"/>
+      <c r="M3" s="3">
+        <v>41480</v>
+      </c>
+      <c r="N3">
+        <v>11.9</v>
+      </c>
+      <c r="O3">
+        <v>11.9</v>
+      </c>
+      <c r="R3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="2:18">
+      <c r="B4" s="12"/>
+      <c r="C4" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="7">
+        <v>1</v>
+      </c>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="8"/>
+      <c r="M4" s="3">
+        <f t="shared" ref="M4:M14" si="0">M3+1</f>
+        <v>41481</v>
+      </c>
+      <c r="O4" s="4">
+        <f t="shared" ref="O4:O13" si="1">O$14-(O$14-O$3)/11*R4</f>
+        <v>13.09090909090909</v>
+      </c>
+      <c r="P4">
+        <f>N4-N3</f>
+        <v>-11.9</v>
+      </c>
+      <c r="Q4" s="4">
+        <f>O4-O3</f>
+        <v>1.1909090909090896</v>
+      </c>
+      <c r="R4">
+        <f>R3-1</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="2:18">
+      <c r="B5" s="12"/>
+      <c r="C5" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="7">
+        <v>1</v>
+      </c>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="8"/>
+      <c r="M5" s="3">
+        <f t="shared" si="0"/>
+        <v>41482</v>
+      </c>
+      <c r="O5" s="4">
+        <f t="shared" si="1"/>
+        <v>14.281818181818181</v>
+      </c>
+      <c r="P5">
+        <f t="shared" ref="P5:P14" si="2">N5-N4</f>
+        <v>0</v>
+      </c>
+      <c r="Q5" s="4">
+        <f t="shared" ref="Q5:Q14" si="3">O5-O4</f>
+        <v>1.1909090909090914</v>
+      </c>
+      <c r="R5">
+        <f t="shared" ref="R5:R14" si="4">R4-1</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18">
+      <c r="B6" s="13"/>
+      <c r="C6" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="9">
+        <v>1</v>
+      </c>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="10"/>
+      <c r="M6" s="3">
+        <f t="shared" si="0"/>
+        <v>41483</v>
+      </c>
+      <c r="O6" s="4">
+        <f t="shared" si="1"/>
+        <v>15.472727272727273</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q6" s="4">
+        <f t="shared" si="3"/>
+        <v>1.1909090909090914</v>
+      </c>
+      <c r="R6">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="2:18">
+      <c r="B7" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="5">
+        <v>1</v>
+      </c>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="6"/>
+      <c r="M7" s="3">
+        <f t="shared" si="0"/>
+        <v>41484</v>
+      </c>
+      <c r="O7" s="4">
+        <f t="shared" si="1"/>
+        <v>16.663636363636364</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q7" s="4">
+        <f t="shared" si="3"/>
+        <v>1.1909090909090914</v>
+      </c>
+      <c r="R7">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="2:18">
+      <c r="B8" s="12"/>
+      <c r="C8" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="7">
+        <v>1</v>
+      </c>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="8"/>
+      <c r="M8" s="3">
+        <f t="shared" si="0"/>
+        <v>41485</v>
+      </c>
+      <c r="O8" s="4">
+        <f t="shared" si="1"/>
+        <v>17.854545454545455</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q8" s="4">
+        <f t="shared" si="3"/>
+        <v>1.1909090909090914</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18">
+      <c r="B9" s="12"/>
+      <c r="C9" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="8">
+        <v>1</v>
+      </c>
+      <c r="M9" s="3">
+        <f t="shared" si="0"/>
+        <v>41486</v>
+      </c>
+      <c r="O9" s="4">
+        <f t="shared" si="1"/>
+        <v>19.045454545454547</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q9" s="4">
+        <f t="shared" si="3"/>
+        <v>1.1909090909090914</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="2:18">
+      <c r="B10" s="13"/>
+      <c r="C10" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="10">
+        <v>1</v>
+      </c>
+      <c r="M10" s="3">
+        <f t="shared" si="0"/>
+        <v>41487</v>
+      </c>
+      <c r="O10" s="4">
+        <f t="shared" si="1"/>
+        <v>20.236363636363635</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q10" s="4">
+        <f t="shared" si="3"/>
+        <v>1.1909090909090878</v>
+      </c>
+      <c r="R10">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18">
+      <c r="B11" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="5">
+        <v>1</v>
+      </c>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="6"/>
+      <c r="M11" s="3">
+        <f t="shared" si="0"/>
+        <v>41488</v>
+      </c>
+      <c r="O11" s="4">
+        <f t="shared" si="1"/>
+        <v>21.427272727272726</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q11" s="4">
+        <f t="shared" si="3"/>
+        <v>1.1909090909090914</v>
+      </c>
+      <c r="R11">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18">
+      <c r="B12" s="12"/>
+      <c r="C12" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="7">
+        <v>1</v>
+      </c>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="8"/>
+      <c r="M12" s="3">
+        <f t="shared" si="0"/>
+        <v>41489</v>
+      </c>
+      <c r="O12" s="4">
+        <f t="shared" si="1"/>
+        <v>22.618181818181817</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q12" s="4">
+        <f t="shared" si="3"/>
+        <v>1.1909090909090914</v>
+      </c>
+      <c r="R12">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18">
+      <c r="B13" s="12"/>
+      <c r="C13" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="7">
+        <v>1</v>
+      </c>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="8"/>
+      <c r="M13" s="3">
+        <f t="shared" si="0"/>
+        <v>41490</v>
+      </c>
+      <c r="O13" s="4">
+        <f t="shared" si="1"/>
+        <v>23.809090909090909</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q13" s="4">
+        <f t="shared" si="3"/>
+        <v>1.1909090909090914</v>
+      </c>
+      <c r="R13">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18">
+      <c r="B14" s="12"/>
+      <c r="C14" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="7">
+        <v>1</v>
+      </c>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="8"/>
+      <c r="M14" s="3">
+        <f t="shared" si="0"/>
+        <v>41491</v>
+      </c>
+      <c r="O14">
+        <v>25</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q14" s="4">
+        <f t="shared" si="3"/>
+        <v>1.1909090909090914</v>
+      </c>
+      <c r="R14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18">
+      <c r="B15" s="12"/>
+      <c r="C15" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7">
+        <v>1</v>
+      </c>
+      <c r="G15" s="8"/>
+    </row>
+    <row r="16" spans="2:18">
+      <c r="B16" s="13"/>
+      <c r="C16" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9">
+        <v>1</v>
+      </c>
+      <c r="G16" s="10"/>
+    </row>
+    <row r="17" spans="2:13">
+      <c r="B17" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5">
+        <v>1</v>
+      </c>
+      <c r="G17" s="6"/>
+    </row>
+    <row r="18" spans="2:13">
+      <c r="B18" s="12"/>
+      <c r="C18" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7">
+        <v>1</v>
+      </c>
+      <c r="G18" s="8"/>
+      <c r="I18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13">
+      <c r="B19" s="12"/>
+      <c r="C19" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="8">
+        <v>1</v>
+      </c>
+      <c r="I19">
+        <f>D29+0.7*E29+0.3*F29</f>
+        <v>11.899999999999999</v>
+      </c>
+      <c r="M19" s="3"/>
+    </row>
+    <row r="20" spans="2:13">
+      <c r="B20" s="13"/>
+      <c r="C20" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="10">
+        <v>1</v>
+      </c>
+      <c r="M20" s="3"/>
+    </row>
+    <row r="21" spans="2:13">
+      <c r="B21" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="6">
+        <v>1</v>
+      </c>
+      <c r="M21" s="3"/>
+    </row>
+    <row r="22" spans="2:13">
+      <c r="B22" s="12"/>
+      <c r="C22" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="8">
+        <v>1</v>
+      </c>
+      <c r="M22" s="3"/>
+    </row>
+    <row r="23" spans="2:13">
+      <c r="B23" s="12"/>
+      <c r="C23" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7">
+        <v>1</v>
+      </c>
+      <c r="F23" s="7"/>
+      <c r="G23" s="8"/>
+    </row>
+    <row r="24" spans="2:13">
+      <c r="B24" s="12"/>
+      <c r="C24" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13">
+      <c r="B25" s="12"/>
+      <c r="C25" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13">
+      <c r="B26" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13">
+      <c r="B27" s="13"/>
+      <c r="C27" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:13">
+      <c r="C29" t="s">
+        <v>62</v>
+      </c>
+      <c r="D29">
+        <f>SUM(D3:D27)</f>
+        <v>10</v>
+      </c>
+      <c r="E29">
+        <f>SUM(E3:E27)</f>
+        <v>1</v>
+      </c>
+      <c r="F29">
+        <f t="shared" ref="F29:G29" si="5">SUM(F3:F27)</f>
+        <v>4</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="I29">
+        <f>SUM(D29:G29)</f>
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="B11:B16"/>
+    <mergeCell ref="B17:B20"/>
+    <mergeCell ref="B21:B25"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <ignoredErrors>
+    <ignoredError sqref="D29:G29" emptyCellReference="1"/>
+  </ignoredErrors>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Some edits to design section.
</commit_message>
<xml_diff>
--- a/_notes/thesis progress.xlsx
+++ b/_notes/thesis progress.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="0" windowWidth="25600" windowHeight="15560" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15560" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -368,7 +368,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -383,12 +383,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -732,8 +733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2018,8 +2019,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:R29"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2084,7 +2085,7 @@
       </c>
     </row>
     <row r="4" spans="2:18">
-      <c r="B4" s="12"/>
+      <c r="B4" s="13"/>
       <c r="C4" s="7" t="s">
         <v>31</v>
       </c>
@@ -2098,16 +2099,19 @@
         <f t="shared" ref="M4:M14" si="0">M3+1</f>
         <v>41481</v>
       </c>
+      <c r="N4">
+        <v>12.6</v>
+      </c>
       <c r="O4" s="4">
         <f t="shared" ref="O4:O13" si="1">O$14-(O$14-O$3)/11*R4</f>
         <v>13.09090909090909</v>
       </c>
       <c r="P4">
         <f>N4-N3</f>
-        <v>-11.9</v>
+        <v>0.69999999999999929</v>
       </c>
       <c r="Q4" s="4">
-        <f>O4-O3</f>
+        <f>O4-N3</f>
         <v>1.1909090909090896</v>
       </c>
       <c r="R4">
@@ -2116,7 +2120,7 @@
       </c>
     </row>
     <row r="5" spans="2:18">
-      <c r="B5" s="12"/>
+      <c r="B5" s="13"/>
       <c r="C5" s="7" t="s">
         <v>32</v>
       </c>
@@ -2130,17 +2134,20 @@
         <f t="shared" si="0"/>
         <v>41482</v>
       </c>
+      <c r="N5">
+        <v>13.3</v>
+      </c>
       <c r="O5" s="4">
         <f t="shared" si="1"/>
         <v>14.281818181818181</v>
       </c>
       <c r="P5">
         <f t="shared" ref="P5:P14" si="2">N5-N4</f>
-        <v>0</v>
+        <v>0.70000000000000107</v>
       </c>
       <c r="Q5" s="4">
-        <f t="shared" ref="Q5:Q14" si="3">O5-O4</f>
-        <v>1.1909090909090914</v>
+        <f t="shared" ref="Q5:Q14" si="3">O5-N4</f>
+        <v>1.6818181818181817</v>
       </c>
       <c r="R5">
         <f t="shared" ref="R5:R14" si="4">R4-1</f>
@@ -2148,7 +2155,7 @@
       </c>
     </row>
     <row r="6" spans="2:18">
-      <c r="B6" s="13"/>
+      <c r="B6" s="12"/>
       <c r="C6" s="9" t="s">
         <v>33</v>
       </c>
@@ -2162,6 +2169,9 @@
         <f t="shared" si="0"/>
         <v>41483</v>
       </c>
+      <c r="N6">
+        <v>13.3</v>
+      </c>
       <c r="O6" s="4">
         <f t="shared" si="1"/>
         <v>15.472727272727273</v>
@@ -2172,7 +2182,7 @@
       </c>
       <c r="Q6" s="4">
         <f t="shared" si="3"/>
-        <v>1.1909090909090914</v>
+        <v>2.172727272727272</v>
       </c>
       <c r="R6">
         <f t="shared" si="4"/>
@@ -2196,17 +2206,20 @@
         <f t="shared" si="0"/>
         <v>41484</v>
       </c>
+      <c r="N7">
+        <v>15.3</v>
+      </c>
       <c r="O7" s="4">
         <f t="shared" si="1"/>
         <v>16.663636363636364</v>
       </c>
       <c r="P7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q7" s="4">
         <f t="shared" si="3"/>
-        <v>1.1909090909090914</v>
+        <v>3.3636363636363633</v>
       </c>
       <c r="R7">
         <f t="shared" si="4"/>
@@ -2214,7 +2227,7 @@
       </c>
     </row>
     <row r="8" spans="2:18">
-      <c r="B8" s="12"/>
+      <c r="B8" s="13"/>
       <c r="C8" s="7" t="s">
         <v>35</v>
       </c>
@@ -2234,11 +2247,11 @@
       </c>
       <c r="P8">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-15.3</v>
       </c>
       <c r="Q8" s="4">
         <f t="shared" si="3"/>
-        <v>1.1909090909090914</v>
+        <v>2.5545454545454547</v>
       </c>
       <c r="R8">
         <f t="shared" si="4"/>
@@ -2246,7 +2259,7 @@
       </c>
     </row>
     <row r="9" spans="2:18">
-      <c r="B9" s="12"/>
+      <c r="B9" s="13"/>
       <c r="C9" s="7" t="s">
         <v>36</v>
       </c>
@@ -2270,7 +2283,7 @@
       </c>
       <c r="Q9" s="4">
         <f t="shared" si="3"/>
-        <v>1.1909090909090914</v>
+        <v>19.045454545454547</v>
       </c>
       <c r="R9">
         <f t="shared" si="4"/>
@@ -2278,7 +2291,7 @@
       </c>
     </row>
     <row r="10" spans="2:18">
-      <c r="B10" s="13"/>
+      <c r="B10" s="12"/>
       <c r="C10" s="9" t="s">
         <v>37</v>
       </c>
@@ -2302,7 +2315,7 @@
       </c>
       <c r="Q10" s="4">
         <f t="shared" si="3"/>
-        <v>1.1909090909090878</v>
+        <v>20.236363636363635</v>
       </c>
       <c r="R10">
         <f t="shared" si="4"/>
@@ -2336,7 +2349,7 @@
       </c>
       <c r="Q11" s="4">
         <f t="shared" si="3"/>
-        <v>1.1909090909090914</v>
+        <v>21.427272727272726</v>
       </c>
       <c r="R11">
         <f t="shared" si="4"/>
@@ -2344,7 +2357,7 @@
       </c>
     </row>
     <row r="12" spans="2:18">
-      <c r="B12" s="12"/>
+      <c r="B12" s="13"/>
       <c r="C12" s="7" t="s">
         <v>41</v>
       </c>
@@ -2368,7 +2381,7 @@
       </c>
       <c r="Q12" s="4">
         <f t="shared" si="3"/>
-        <v>1.1909090909090914</v>
+        <v>22.618181818181817</v>
       </c>
       <c r="R12">
         <f t="shared" si="4"/>
@@ -2376,7 +2389,7 @@
       </c>
     </row>
     <row r="13" spans="2:18">
-      <c r="B13" s="12"/>
+      <c r="B13" s="13"/>
       <c r="C13" s="7" t="s">
         <v>42</v>
       </c>
@@ -2400,7 +2413,7 @@
       </c>
       <c r="Q13" s="4">
         <f t="shared" si="3"/>
-        <v>1.1909090909090914</v>
+        <v>23.809090909090909</v>
       </c>
       <c r="R13">
         <f t="shared" si="4"/>
@@ -2408,7 +2421,7 @@
       </c>
     </row>
     <row r="14" spans="2:18">
-      <c r="B14" s="12"/>
+      <c r="B14" s="13"/>
       <c r="C14" s="7" t="s">
         <v>43</v>
       </c>
@@ -2431,7 +2444,7 @@
       </c>
       <c r="Q14" s="4">
         <f t="shared" si="3"/>
-        <v>1.1909090909090914</v>
+        <v>25</v>
       </c>
       <c r="R14">
         <f t="shared" si="4"/>
@@ -2439,7 +2452,7 @@
       </c>
     </row>
     <row r="15" spans="2:18">
-      <c r="B15" s="12"/>
+      <c r="B15" s="13"/>
       <c r="C15" s="7" t="s">
         <v>44</v>
       </c>
@@ -2451,7 +2464,7 @@
       <c r="G15" s="8"/>
     </row>
     <row r="16" spans="2:18">
-      <c r="B16" s="13"/>
+      <c r="B16" s="12"/>
       <c r="C16" s="9" t="s">
         <v>45</v>
       </c>
@@ -2469,56 +2482,56 @@
       <c r="C17" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D17" s="5"/>
+      <c r="D17" s="5">
+        <v>1</v>
+      </c>
       <c r="E17" s="5"/>
-      <c r="F17" s="5">
-        <v>1</v>
-      </c>
+      <c r="F17" s="5"/>
       <c r="G17" s="6"/>
     </row>
     <row r="18" spans="2:13">
-      <c r="B18" s="12"/>
+      <c r="B18" s="13"/>
       <c r="C18" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D18" s="7"/>
+      <c r="D18" s="14">
+        <v>1</v>
+      </c>
       <c r="E18" s="7"/>
-      <c r="F18" s="7">
-        <v>1</v>
-      </c>
+      <c r="F18" s="7"/>
       <c r="G18" s="8"/>
       <c r="I18" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="19" spans="2:13">
-      <c r="B19" s="12"/>
+      <c r="B19" s="13"/>
       <c r="C19" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D19" s="7"/>
+      <c r="D19" s="14">
+        <v>1</v>
+      </c>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
-      <c r="G19" s="8">
-        <v>1</v>
-      </c>
+      <c r="G19" s="8"/>
       <c r="I19">
         <f>D29+0.7*E29+0.3*F29</f>
-        <v>11.899999999999999</v>
+        <v>15.299999999999999</v>
       </c>
       <c r="M19" s="3"/>
     </row>
     <row r="20" spans="2:13">
-      <c r="B20" s="13"/>
+      <c r="B20" s="12"/>
       <c r="C20" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="D20" s="9"/>
+      <c r="D20" s="9">
+        <v>1</v>
+      </c>
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
-      <c r="G20" s="10">
-        <v>1</v>
-      </c>
+      <c r="G20" s="10"/>
       <c r="M20" s="3"/>
     </row>
     <row r="21" spans="2:13">
@@ -2537,7 +2550,7 @@
       <c r="M21" s="3"/>
     </row>
     <row r="22" spans="2:13">
-      <c r="B22" s="12"/>
+      <c r="B22" s="13"/>
       <c r="C22" s="7" t="s">
         <v>52</v>
       </c>
@@ -2550,7 +2563,7 @@
       <c r="M22" s="3"/>
     </row>
     <row r="23" spans="2:13">
-      <c r="B23" s="12"/>
+      <c r="B23" s="13"/>
       <c r="C23" s="7" t="s">
         <v>53</v>
       </c>
@@ -2562,7 +2575,7 @@
       <c r="G23" s="8"/>
     </row>
     <row r="24" spans="2:13">
-      <c r="B24" s="12"/>
+      <c r="B24" s="13"/>
       <c r="C24" s="7" t="s">
         <v>51</v>
       </c>
@@ -2574,7 +2587,7 @@
       </c>
     </row>
     <row r="25" spans="2:13">
-      <c r="B25" s="12"/>
+      <c r="B25" s="13"/>
       <c r="C25" s="7" t="s">
         <v>54</v>
       </c>
@@ -2600,7 +2613,7 @@
       </c>
     </row>
     <row r="27" spans="2:13">
-      <c r="B27" s="13"/>
+      <c r="B27" s="12"/>
       <c r="C27" s="9" t="s">
         <v>56</v>
       </c>
@@ -2617,7 +2630,7 @@
       </c>
       <c r="D29">
         <f>SUM(D3:D27)</f>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E29">
         <f>SUM(E3:E27)</f>
@@ -2625,11 +2638,11 @@
       </c>
       <c r="F29">
         <f t="shared" ref="F29:G29" si="5">SUM(F3:F27)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G29">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I29">
         <f>SUM(D29:G29)</f>

</xml_diff>

<commit_message>
2nd round of edits to chapter 4.
</commit_message>
<xml_diff>
--- a/_notes/thesis progress.xlsx
+++ b/_notes/thesis progress.xlsx
@@ -380,6 +380,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -389,7 +390,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2059,7 +2059,7 @@
       </c>
     </row>
     <row r="3" spans="2:18">
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="12" t="s">
         <v>57</v>
       </c>
       <c r="C3" s="5" t="s">
@@ -2085,7 +2085,7 @@
       </c>
     </row>
     <row r="4" spans="2:18">
-      <c r="B4" s="13"/>
+      <c r="B4" s="14"/>
       <c r="C4" s="7" t="s">
         <v>31</v>
       </c>
@@ -2120,7 +2120,7 @@
       </c>
     </row>
     <row r="5" spans="2:18">
-      <c r="B5" s="13"/>
+      <c r="B5" s="14"/>
       <c r="C5" s="7" t="s">
         <v>32</v>
       </c>
@@ -2155,7 +2155,7 @@
       </c>
     </row>
     <row r="6" spans="2:18">
-      <c r="B6" s="12"/>
+      <c r="B6" s="13"/>
       <c r="C6" s="9" t="s">
         <v>33</v>
       </c>
@@ -2190,7 +2190,7 @@
       </c>
     </row>
     <row r="7" spans="2:18">
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="12" t="s">
         <v>38</v>
       </c>
       <c r="C7" s="5" t="s">
@@ -2227,7 +2227,7 @@
       </c>
     </row>
     <row r="8" spans="2:18">
-      <c r="B8" s="13"/>
+      <c r="B8" s="14"/>
       <c r="C8" s="7" t="s">
         <v>35</v>
       </c>
@@ -2259,7 +2259,7 @@
       </c>
     </row>
     <row r="9" spans="2:18">
-      <c r="B9" s="13"/>
+      <c r="B9" s="14"/>
       <c r="C9" s="7" t="s">
         <v>36</v>
       </c>
@@ -2291,7 +2291,7 @@
       </c>
     </row>
     <row r="10" spans="2:18">
-      <c r="B10" s="12"/>
+      <c r="B10" s="13"/>
       <c r="C10" s="9" t="s">
         <v>37</v>
       </c>
@@ -2323,7 +2323,7 @@
       </c>
     </row>
     <row r="11" spans="2:18">
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="12" t="s">
         <v>39</v>
       </c>
       <c r="C11" s="5" t="s">
@@ -2357,7 +2357,7 @@
       </c>
     </row>
     <row r="12" spans="2:18">
-      <c r="B12" s="13"/>
+      <c r="B12" s="14"/>
       <c r="C12" s="7" t="s">
         <v>41</v>
       </c>
@@ -2389,7 +2389,7 @@
       </c>
     </row>
     <row r="13" spans="2:18">
-      <c r="B13" s="13"/>
+      <c r="B13" s="14"/>
       <c r="C13" s="7" t="s">
         <v>42</v>
       </c>
@@ -2421,7 +2421,7 @@
       </c>
     </row>
     <row r="14" spans="2:18">
-      <c r="B14" s="13"/>
+      <c r="B14" s="14"/>
       <c r="C14" s="7" t="s">
         <v>43</v>
       </c>
@@ -2452,7 +2452,7 @@
       </c>
     </row>
     <row r="15" spans="2:18">
-      <c r="B15" s="13"/>
+      <c r="B15" s="14"/>
       <c r="C15" s="7" t="s">
         <v>44</v>
       </c>
@@ -2464,7 +2464,7 @@
       <c r="G15" s="8"/>
     </row>
     <row r="16" spans="2:18">
-      <c r="B16" s="12"/>
+      <c r="B16" s="13"/>
       <c r="C16" s="9" t="s">
         <v>45</v>
       </c>
@@ -2476,7 +2476,7 @@
       <c r="G16" s="10"/>
     </row>
     <row r="17" spans="2:13">
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="12" t="s">
         <v>24</v>
       </c>
       <c r="C17" s="5" t="s">
@@ -2490,11 +2490,11 @@
       <c r="G17" s="6"/>
     </row>
     <row r="18" spans="2:13">
-      <c r="B18" s="13"/>
+      <c r="B18" s="14"/>
       <c r="C18" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D18" s="14">
+      <c r="D18" s="11">
         <v>1</v>
       </c>
       <c r="E18" s="7"/>
@@ -2505,11 +2505,11 @@
       </c>
     </row>
     <row r="19" spans="2:13">
-      <c r="B19" s="13"/>
+      <c r="B19" s="14"/>
       <c r="C19" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D19" s="14">
+      <c r="D19" s="11">
         <v>1</v>
       </c>
       <c r="E19" s="7"/>
@@ -2522,7 +2522,7 @@
       <c r="M19" s="3"/>
     </row>
     <row r="20" spans="2:13">
-      <c r="B20" s="12"/>
+      <c r="B20" s="13"/>
       <c r="C20" s="9" t="s">
         <v>49</v>
       </c>
@@ -2535,7 +2535,7 @@
       <c r="M20" s="3"/>
     </row>
     <row r="21" spans="2:13">
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="12" t="s">
         <v>50</v>
       </c>
       <c r="C21" s="5" t="s">
@@ -2550,7 +2550,7 @@
       <c r="M21" s="3"/>
     </row>
     <row r="22" spans="2:13">
-      <c r="B22" s="13"/>
+      <c r="B22" s="14"/>
       <c r="C22" s="7" t="s">
         <v>52</v>
       </c>
@@ -2563,7 +2563,7 @@
       <c r="M22" s="3"/>
     </row>
     <row r="23" spans="2:13">
-      <c r="B23" s="13"/>
+      <c r="B23" s="14"/>
       <c r="C23" s="7" t="s">
         <v>53</v>
       </c>
@@ -2575,7 +2575,7 @@
       <c r="G23" s="8"/>
     </row>
     <row r="24" spans="2:13">
-      <c r="B24" s="13"/>
+      <c r="B24" s="14"/>
       <c r="C24" s="7" t="s">
         <v>51</v>
       </c>
@@ -2587,7 +2587,7 @@
       </c>
     </row>
     <row r="25" spans="2:13">
-      <c r="B25" s="13"/>
+      <c r="B25" s="14"/>
       <c r="C25" s="7" t="s">
         <v>54</v>
       </c>
@@ -2599,7 +2599,7 @@
       </c>
     </row>
     <row r="26" spans="2:13">
-      <c r="B26" s="11" t="s">
+      <c r="B26" s="12" t="s">
         <v>22</v>
       </c>
       <c r="C26" s="5" t="s">
@@ -2613,7 +2613,7 @@
       </c>
     </row>
     <row r="27" spans="2:13">
-      <c r="B27" s="12"/>
+      <c r="B27" s="13"/>
       <c r="C27" s="9" t="s">
         <v>56</v>
       </c>

</xml_diff>